<commit_message>
plotted suspended d15 and just 2017 sinking d15
</commit_message>
<xml_diff>
--- a/data/flux/2012-pumps.xlsx
+++ b/data/flux/2012-pumps.xlsx
@@ -243,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -267,16 +267,23 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -322,12 +329,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -335,7 +342,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,2454 +369,2451 @@
   </sheetPr>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>-22.22</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>221.07</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>0.22</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>18.41</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="3" t="n">
         <v>8.55</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="L2" s="3" t="n">
         <v>35.59</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="3" t="n">
         <v>2.54</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="3" t="n">
         <v>7.246601298</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="2" t="n">
+      <c r="P2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="3" t="n">
         <v>36.16</v>
       </c>
-      <c r="R2" s="2" t="n">
+      <c r="R2" s="3" t="n">
         <v>7.232</v>
       </c>
-      <c r="S2" s="2" t="n">
+      <c r="S2" s="3" t="n">
         <v>3.056849566</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="C3" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>-25.03</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <v>425.41</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>0.43</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>35.42</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="3" t="n">
         <v>9.2</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="L3" s="3" t="n">
         <v>63.79</v>
       </c>
-      <c r="M3" s="2" t="n">
+      <c r="M3" s="3" t="n">
         <v>4.55</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="3" t="n">
         <v>7.779493991</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="2" t="n">
+      <c r="P3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="3" t="n">
         <v>38.23</v>
       </c>
-      <c r="R3" s="2" t="n">
+      <c r="R3" s="3" t="n">
         <v>7.646</v>
       </c>
-      <c r="S3" s="2" t="n">
+      <c r="S3" s="3" t="n">
         <v>5.563860816</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>-23.95</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="3" t="n">
         <v>294.27</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="3" t="n">
         <v>0.29</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="n">
         <v>24.5</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="3" t="n">
         <v>8.16</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="3" t="n">
         <v>53.66</v>
       </c>
-      <c r="M4" s="2" t="n">
+      <c r="M4" s="3" t="n">
         <v>3.83</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="O4" s="3" t="n">
         <v>6.397734712</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="2" t="n">
+      <c r="P4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="3" t="n">
         <v>36.58</v>
       </c>
-      <c r="R4" s="2" t="n">
+      <c r="R4" s="3" t="n">
         <v>7.316</v>
       </c>
-      <c r="S4" s="2" t="n">
+      <c r="S4" s="3" t="n">
         <v>4.022297866</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D5" s="1" t="n">
+      <c r="C5" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>-26.13</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="n">
         <v>348.64</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v>0.35</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="3" t="n">
         <v>29.03</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="3" t="n">
         <v>8.64</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="L5" s="3" t="n">
         <v>64.69</v>
       </c>
-      <c r="M5" s="2" t="n">
+      <c r="M5" s="3" t="n">
         <v>4.62</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="O5" s="3" t="n">
         <v>6.287227036</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5" s="2" t="n">
+      <c r="P5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="3" t="n">
         <v>36.5</v>
       </c>
-      <c r="R5" s="2" t="n">
+      <c r="R5" s="3" t="n">
         <v>7.3</v>
       </c>
-      <c r="S5" s="2" t="n">
+      <c r="S5" s="3" t="n">
         <v>4.775879861</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D6" s="1" t="n">
+      <c r="C6" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>560</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>560</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="n">
         <v>-22.85</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="3" t="n">
         <v>159.43</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="3" t="n">
         <v>0.16</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <v>13.28</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="3" t="n">
         <v>9.79</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="3" t="n">
         <v>24.14</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="M6" s="3" t="n">
         <v>1.72</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="O6" s="3" t="n">
         <v>7.703421613</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q6" s="2" t="n">
+      <c r="P6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" s="3" t="n">
         <v>37.64</v>
       </c>
-      <c r="R6" s="2" t="n">
+      <c r="R6" s="3" t="n">
         <v>7.528</v>
       </c>
-      <c r="S6" s="2" t="n">
+      <c r="S6" s="3" t="n">
         <v>2.11787073</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D7" s="1" t="n">
+      <c r="C7" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>650</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>650</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>-23.02</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="3" t="n">
         <v>122.57</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="3" t="n">
         <v>0.12</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="3" t="n">
         <v>10.21</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="3" t="n">
         <v>10.04</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="L7" s="3" t="n">
         <v>18.91</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="M7" s="3" t="n">
         <v>1.35</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O7" s="3" t="n">
         <v>7.561291279</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q7" s="2" t="n">
+      <c r="P7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="3" t="n">
         <v>34.13</v>
       </c>
-      <c r="R7" s="2" t="n">
+      <c r="R7" s="3" t="n">
         <v>6.826</v>
       </c>
-      <c r="S7" s="2" t="n">
+      <c r="S7" s="3" t="n">
         <v>1.795606494</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D8" s="1" t="n">
+      <c r="C8" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>-24.96</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="3" t="n">
         <v>232.34</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="3" t="n">
         <v>0.23</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="3" t="n">
         <v>19.35</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="3" t="n">
         <v>9.77</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="L8" s="3" t="n">
         <v>33.25</v>
       </c>
-      <c r="M8" s="2" t="n">
+      <c r="M8" s="3" t="n">
         <v>2.37</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="O8" s="3" t="n">
         <v>8.152265613</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q8" s="2" t="n">
+      <c r="P8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="3" t="n">
         <v>38.62</v>
       </c>
-      <c r="R8" s="2" t="n">
+      <c r="R8" s="3" t="n">
         <v>7.724</v>
       </c>
-      <c r="S8" s="2" t="n">
+      <c r="S8" s="3" t="n">
         <v>3.008016553</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D9" s="1" t="n">
+      <c r="C9" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>1100</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>1100</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>-23.38</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="3" t="n">
         <v>51.97</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="3" t="n">
         <v>4.33</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="3" t="n">
         <v>9.43</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="L9" s="3" t="n">
         <v>7.35</v>
       </c>
-      <c r="M9" s="2" t="n">
+      <c r="M9" s="3" t="n">
         <v>0.52</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="O9" s="3" t="n">
         <v>8.244890617</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q9" s="2" t="n">
+      <c r="P9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="3" t="n">
         <v>35.53</v>
       </c>
-      <c r="R9" s="2" t="n">
+      <c r="R9" s="3" t="n">
         <v>7.106</v>
       </c>
-      <c r="S9" s="2" t="n">
-        <v>0.7313111055</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D10" s="1" t="n">
+      <c r="C10" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>170</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>170</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <v>-24.96</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <v>236.09</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="3" t="n">
         <v>0.24</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="3" t="n">
         <v>19.66</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="3" t="n">
         <v>9.6</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="L10" s="3" t="n">
         <v>33.25</v>
       </c>
-      <c r="M10" s="2" t="n">
+      <c r="M10" s="3" t="n">
         <v>2.37</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="O10" s="3" t="n">
         <v>8.284035519</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10" s="2" t="n">
+      <c r="P10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="3" t="n">
         <v>37.93</v>
       </c>
-      <c r="R10" s="2" t="n">
+      <c r="R10" s="3" t="n">
         <v>7.586</v>
       </c>
-      <c r="S10" s="2" t="n">
+      <c r="S10" s="3" t="n">
         <v>3.11224143</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D11" s="1" t="n">
+      <c r="C11" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D11" s="2" t="n">
         <v>195</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>195</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>-24.77</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <v>134.8</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="3" t="n">
         <v>11.22</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="3" t="n">
         <v>9.49</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="L11" s="3" t="n">
         <v>20.17</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="M11" s="3" t="n">
         <v>1.44</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="O11" s="3" t="n">
         <v>7.794752887</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q11" s="2" t="n">
+      <c r="P11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="3" t="n">
         <v>36.22</v>
       </c>
-      <c r="R11" s="2" t="n">
+      <c r="R11" s="3" t="n">
         <v>7.244</v>
       </c>
-      <c r="S11" s="2" t="n">
+      <c r="S11" s="3" t="n">
         <v>1.860802302</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D12" s="1" t="n">
+      <c r="C12" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="E12" s="3" t="n">
+      <c r="E12" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>-25.39</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <v>374.87</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="3" t="n">
         <v>0.37</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="3" t="n">
         <v>31.21</v>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="K12" s="3" t="n">
         <v>8.71</v>
       </c>
-      <c r="L12" s="2" t="n">
+      <c r="L12" s="3" t="n">
         <v>53.57</v>
       </c>
-      <c r="M12" s="2" t="n">
+      <c r="M12" s="3" t="n">
         <v>3.82</v>
       </c>
-      <c r="O12" s="2" t="n">
+      <c r="O12" s="3" t="n">
         <v>8.163609669</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12" s="2" t="n">
+      <c r="P12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="3" t="n">
         <v>34.47</v>
       </c>
-      <c r="R12" s="2" t="n">
+      <c r="R12" s="3" t="n">
         <v>6.894</v>
       </c>
-      <c r="S12" s="2" t="n">
+      <c r="S12" s="3" t="n">
         <v>5.437578114</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D13" s="1" t="n">
+      <c r="C13" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D13" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="E13" s="3" t="n">
+      <c r="E13" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <v>-23.03</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <v>176.92</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="3" t="n">
         <v>0.18</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="I13" s="3" t="n">
         <v>14.73</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="K13" s="3" t="n">
         <v>9.21</v>
       </c>
-      <c r="L13" s="2" t="n">
+      <c r="L13" s="3" t="n">
         <v>28.29</v>
       </c>
-      <c r="M13" s="2" t="n">
+      <c r="M13" s="3" t="n">
         <v>2.02</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="O13" s="3" t="n">
         <v>7.294956205</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q13" s="2" t="n">
+      <c r="P13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="3" t="n">
         <v>30.32</v>
       </c>
-      <c r="R13" s="2" t="n">
+      <c r="R13" s="3" t="n">
         <v>6.064</v>
       </c>
-      <c r="S13" s="2" t="n">
+      <c r="S13" s="3" t="n">
         <v>2.917495266</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D14" s="1" t="n">
+      <c r="C14" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="E14" s="3" t="n">
+      <c r="E14" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>-25.04</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <v>260.5</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>0.26</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <v>21.69</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="3" t="n">
         <v>9.38</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="L14" s="3" t="n">
         <v>43.32</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="M14" s="3" t="n">
         <v>3.09</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="O14" s="3" t="n">
         <v>7.014008328</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q14" s="2" t="n">
+      <c r="P14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="3" t="n">
         <v>34.48</v>
       </c>
-      <c r="R14" s="2" t="n">
+      <c r="R14" s="3" t="n">
         <v>6.896</v>
       </c>
-      <c r="S14" s="2" t="n">
+      <c r="S14" s="3" t="n">
         <v>3.777534217</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D15" s="1" t="n">
+      <c r="C15" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <v>-23.94</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <v>453.47</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <v>0.45</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="3" t="n">
         <v>37.76</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="K15" s="3" t="n">
         <v>9.43</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="L15" s="3" t="n">
         <v>74</v>
       </c>
-      <c r="M15" s="2" t="n">
+      <c r="M15" s="3" t="n">
         <v>5.28</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="O15" s="3" t="n">
         <v>7.148785534</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="2" t="n">
+      <c r="P15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="3" t="n">
         <v>34.4</v>
       </c>
-      <c r="R15" s="2" t="n">
+      <c r="R15" s="3" t="n">
         <v>6.88</v>
       </c>
-      <c r="S15" s="2" t="n">
+      <c r="S15" s="3" t="n">
         <v>6.59119087</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D16" s="1" t="n">
+      <c r="C16" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D16" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="4" t="n">
         <v>105</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <v>-23.32</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <v>151.91</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="H16" s="3" t="n">
         <v>0.15</v>
       </c>
-      <c r="I16" s="2" t="n">
+      <c r="I16" s="3" t="n">
         <v>12.65</v>
       </c>
-      <c r="K16" s="2" t="n">
+      <c r="K16" s="3" t="n">
         <v>11.78</v>
       </c>
-      <c r="L16" s="2" t="n">
+      <c r="L16" s="3" t="n">
         <v>27.57</v>
       </c>
-      <c r="M16" s="2" t="n">
+      <c r="M16" s="3" t="n">
         <v>1.97</v>
       </c>
-      <c r="O16" s="2" t="n">
+      <c r="O16" s="3" t="n">
         <v>6.427741962</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="2" t="n">
+      <c r="P16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="3" t="n">
         <v>34.79</v>
       </c>
-      <c r="R16" s="2" t="n">
+      <c r="R16" s="3" t="n">
         <v>6.958</v>
       </c>
-      <c r="S16" s="2" t="n">
+      <c r="S16" s="3" t="n">
         <v>2.183267952</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D17" s="1" t="n">
+      <c r="C17" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D17" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="E17" s="3" t="n">
+      <c r="E17" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="3" t="n">
         <v>-25.69</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="3" t="n">
         <v>298.02</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="H17" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="I17" s="3" t="n">
         <v>24.81</v>
       </c>
-      <c r="K17" s="2" t="n">
+      <c r="K17" s="3" t="n">
         <v>9.4</v>
       </c>
-      <c r="L17" s="2" t="n">
+      <c r="L17" s="3" t="n">
         <v>54.55</v>
       </c>
-      <c r="M17" s="2" t="n">
+      <c r="M17" s="3" t="n">
         <v>3.89</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="O17" s="3" t="n">
         <v>6.372689752</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="2" t="n">
+      <c r="P17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="3" t="n">
         <v>36.27</v>
       </c>
-      <c r="R17" s="2" t="n">
+      <c r="R17" s="3" t="n">
         <v>7.254</v>
       </c>
-      <c r="S17" s="2" t="n">
+      <c r="S17" s="3" t="n">
         <v>4.108389076</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D18" s="1" t="n">
+      <c r="C18" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D18" s="2" t="n">
         <v>155</v>
       </c>
-      <c r="E18" s="3" t="n">
+      <c r="E18" s="4" t="n">
         <v>155</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <v>-25.08</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="3" t="n">
         <v>305.52</v>
       </c>
-      <c r="H18" s="2" t="n">
+      <c r="H18" s="3" t="n">
         <v>0.31</v>
       </c>
-      <c r="I18" s="2" t="n">
+      <c r="I18" s="3" t="n">
         <v>25.44</v>
       </c>
-      <c r="K18" s="2" t="n">
+      <c r="K18" s="3" t="n">
         <v>9.66</v>
       </c>
-      <c r="L18" s="2" t="n">
+      <c r="L18" s="3" t="n">
         <v>43.59</v>
       </c>
-      <c r="M18" s="2" t="n">
+      <c r="M18" s="3" t="n">
         <v>3.11</v>
       </c>
-      <c r="O18" s="2" t="n">
+      <c r="O18" s="3" t="n">
         <v>8.175433939</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="2" t="n">
+      <c r="P18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="3" t="n">
         <v>35.33</v>
       </c>
-      <c r="R18" s="2" t="n">
+      <c r="R18" s="3" t="n">
         <v>7.066</v>
       </c>
-      <c r="S18" s="2" t="n">
+      <c r="S18" s="3" t="n">
         <v>4.323864172</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D19" s="1" t="n">
+      <c r="C19" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>710</v>
       </c>
-      <c r="E19" s="3" t="n">
+      <c r="E19" s="4" t="n">
         <v>710</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="3" t="n">
         <v>-22.62</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="3" t="n">
         <v>112.78</v>
       </c>
-      <c r="H19" s="2" t="n">
+      <c r="H19" s="3" t="n">
         <v>0.11</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="I19" s="3" t="n">
         <v>9.39</v>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="K19" s="3" t="n">
         <v>9.62</v>
       </c>
-      <c r="L19" s="2" t="n">
+      <c r="L19" s="3" t="n">
         <v>16.74</v>
       </c>
-      <c r="M19" s="2" t="n">
+      <c r="M19" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="2" t="n">
+      <c r="O19" s="3" t="n">
         <v>7.858187715</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="2" t="n">
+      <c r="P19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="3" t="n">
         <v>34.29</v>
       </c>
-      <c r="R19" s="2" t="n">
+      <c r="R19" s="3" t="n">
         <v>6.858</v>
       </c>
-      <c r="S19" s="2" t="n">
+      <c r="S19" s="3" t="n">
         <v>1.644552723</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D20" s="1" t="n">
+      <c r="C20" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D20" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="4" t="n">
         <v>65</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="3" t="n">
         <v>-23.05</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="3" t="n">
         <v>129.91</v>
       </c>
-      <c r="H20" s="2" t="n">
+      <c r="H20" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I20" s="2" t="n">
+      <c r="I20" s="3" t="n">
         <v>10.82</v>
       </c>
-      <c r="K20" s="2" t="n">
+      <c r="K20" s="3" t="n">
         <v>7.72</v>
       </c>
-      <c r="L20" s="2" t="n">
+      <c r="L20" s="3" t="n">
         <v>22.97</v>
       </c>
-      <c r="M20" s="2" t="n">
+      <c r="M20" s="3" t="n">
         <v>1.64</v>
       </c>
-      <c r="O20" s="2" t="n">
+      <c r="O20" s="3" t="n">
         <v>6.597143684</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="2" t="n">
+      <c r="P20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="3" t="n">
         <v>34.27</v>
       </c>
-      <c r="R20" s="2" t="n">
+      <c r="R20" s="3" t="n">
         <v>6.854</v>
       </c>
-      <c r="S20" s="2" t="n">
+      <c r="S20" s="3" t="n">
         <v>1.895323519</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D21" s="1" t="n">
+      <c r="C21" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D21" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="3" t="n">
         <v>-22.29</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="3" t="n">
         <v>221.07</v>
       </c>
-      <c r="H21" s="2" t="n">
+      <c r="H21" s="3" t="n">
         <v>0.22</v>
       </c>
-      <c r="I21" s="2" t="n">
+      <c r="I21" s="3" t="n">
         <v>18.41</v>
       </c>
-      <c r="K21" s="2" t="n">
+      <c r="K21" s="3" t="n">
         <v>8.58</v>
       </c>
-      <c r="L21" s="2" t="n">
+      <c r="L21" s="3" t="n">
         <v>35.68</v>
       </c>
-      <c r="M21" s="2" t="n">
+      <c r="M21" s="3" t="n">
         <v>2.55</v>
       </c>
-      <c r="O21" s="2" t="n">
+      <c r="O21" s="3" t="n">
         <v>7.228315442</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="2" t="n">
+      <c r="P21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="3" t="n">
         <v>38.23</v>
       </c>
-      <c r="R21" s="2" t="n">
+      <c r="R21" s="3" t="n">
         <v>7.646</v>
       </c>
-      <c r="S21" s="2" t="n">
+      <c r="S21" s="3" t="n">
         <v>2.891333516</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D22" s="1" t="n">
+      <c r="C22" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D22" s="2" t="n">
         <v>1000</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="3" t="n">
         <v>-22.86</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="3" t="n">
         <v>132.54</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="H22" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I22" s="2" t="n">
+      <c r="I22" s="3" t="n">
         <v>11.04</v>
       </c>
-      <c r="K22" s="2" t="n">
+      <c r="K22" s="3" t="n">
         <v>11.11</v>
       </c>
-      <c r="L22" s="2" t="n">
+      <c r="L22" s="3" t="n">
         <v>17.74</v>
       </c>
-      <c r="M22" s="2" t="n">
+      <c r="M22" s="3" t="n">
         <v>1.27</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O22" s="2" t="n">
+      <c r="O22" s="3" t="n">
         <v>8.717487898</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q22" s="2" t="n">
+      <c r="P22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="3" t="n">
         <v>34.21</v>
       </c>
-      <c r="R22" s="2" t="n">
+      <c r="R22" s="3" t="n">
         <v>6.842</v>
       </c>
-      <c r="S22" s="2" t="n">
+      <c r="S22" s="3" t="n">
         <v>1.937140704</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="C23" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D23" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="E23" s="3" t="n">
+      <c r="E23" s="4" t="n">
         <v>80</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="3" t="n">
         <v>-25.45</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="3" t="n">
         <v>260.5</v>
       </c>
-      <c r="H23" s="2" t="n">
+      <c r="H23" s="3" t="n">
         <v>0.26</v>
       </c>
-      <c r="I23" s="2" t="n">
+      <c r="I23" s="3" t="n">
         <v>21.69</v>
       </c>
-      <c r="K23" s="2" t="n">
+      <c r="K23" s="3" t="n">
         <v>9.55</v>
       </c>
-      <c r="L23" s="2" t="n">
+      <c r="L23" s="3" t="n">
         <v>38.11</v>
       </c>
-      <c r="M23" s="2" t="n">
+      <c r="M23" s="3" t="n">
         <v>2.72</v>
       </c>
-      <c r="O23" s="2" t="n">
+      <c r="O23" s="3" t="n">
         <v>7.974280006</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="2" t="n">
+      <c r="P23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="3" t="n">
         <v>33.8</v>
       </c>
-      <c r="R23" s="2" t="n">
+      <c r="R23" s="3" t="n">
         <v>6.76</v>
       </c>
-      <c r="S23" s="2" t="n">
+      <c r="S23" s="3" t="n">
         <v>3.853531947</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D24" s="1" t="n">
+      <c r="C24" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D24" s="2" t="n">
         <v>800</v>
       </c>
-      <c r="E24" s="3" t="n">
+      <c r="E24" s="4" t="n">
         <v>800</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="3" t="n">
         <v>-23.04</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="3" t="n">
         <v>70.43</v>
       </c>
-      <c r="H24" s="2" t="n">
+      <c r="H24" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="I24" s="2" t="n">
+      <c r="I24" s="3" t="n">
         <v>5.86</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="2" t="n">
+      <c r="K24" s="3" t="n">
         <v>10.47</v>
       </c>
-      <c r="L24" s="2" t="n">
+      <c r="L24" s="3" t="n">
         <v>9.78</v>
       </c>
-      <c r="M24" s="2" t="n">
+      <c r="M24" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="2" t="n">
+      <c r="O24" s="3" t="n">
         <v>8.3959214</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q24" s="2" t="n">
+      <c r="P24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="3" t="n">
         <v>31.89</v>
       </c>
-      <c r="R24" s="2" t="n">
+      <c r="R24" s="3" t="n">
         <v>6.378</v>
       </c>
-      <c r="S24" s="2" t="n">
+      <c r="S24" s="3" t="n">
         <v>1.104202623</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D25" s="1" t="n">
+      <c r="C25" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="3" t="n">
         <v>-23.45</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="3" t="n">
         <v>284.89</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="3" t="n">
         <v>0.28</v>
       </c>
-      <c r="I25" s="2" t="n">
+      <c r="I25" s="3" t="n">
         <v>23.72</v>
       </c>
-      <c r="K25" s="2" t="n">
+      <c r="K25" s="3" t="n">
         <v>10.01</v>
       </c>
-      <c r="L25" s="2" t="n">
+      <c r="L25" s="3" t="n">
         <v>39.1</v>
       </c>
-      <c r="M25" s="2" t="n">
+      <c r="M25" s="3" t="n">
         <v>2.79</v>
       </c>
-      <c r="O25" s="2" t="n">
+      <c r="O25" s="3" t="n">
         <v>8.500212605</v>
       </c>
-      <c r="P25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q25" s="2" t="n">
+      <c r="P25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="3" t="n">
         <v>32.85</v>
       </c>
-      <c r="R25" s="2" t="n">
+      <c r="R25" s="3" t="n">
         <v>6.57</v>
       </c>
-      <c r="S25" s="2" t="n">
+      <c r="S25" s="3" t="n">
         <v>4.336257501</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D26" s="1" t="n">
+      <c r="C26" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D26" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="E26" s="3" t="n">
+      <c r="E26" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="3" t="n">
         <v>-24.95</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="3" t="n">
         <v>380.49</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="H26" s="3" t="n">
         <v>0.38</v>
       </c>
-      <c r="I26" s="2" t="n">
+      <c r="I26" s="3" t="n">
         <v>31.68</v>
       </c>
-      <c r="K26" s="2" t="n">
+      <c r="K26" s="3" t="n">
         <v>9.64</v>
       </c>
-      <c r="L26" s="2" t="n">
+      <c r="L26" s="3" t="n">
         <v>51.86</v>
       </c>
-      <c r="M26" s="2" t="n">
+      <c r="M26" s="3" t="n">
         <v>3.7</v>
       </c>
-      <c r="O26" s="2" t="n">
+      <c r="O26" s="3" t="n">
         <v>8.55849593</v>
       </c>
-      <c r="P26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q26" s="2" t="n">
+      <c r="P26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="3" t="n">
         <v>34.35</v>
       </c>
-      <c r="R26" s="2" t="n">
+      <c r="R26" s="3" t="n">
         <v>6.87</v>
       </c>
-      <c r="S26" s="2" t="n">
+      <c r="S26" s="3" t="n">
         <v>5.538357627</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D27" s="1" t="n">
+      <c r="C27" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D27" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="E27" s="4" t="n">
         <v>125</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="3" t="n">
         <v>-24.96</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="3" t="n">
         <v>258.62</v>
       </c>
-      <c r="H27" s="2" t="n">
+      <c r="H27" s="3" t="n">
         <v>0.26</v>
       </c>
-      <c r="I27" s="2" t="n">
+      <c r="I27" s="3" t="n">
         <v>21.53</v>
       </c>
-      <c r="K27" s="2" t="n">
+      <c r="K27" s="3" t="n">
         <v>9.8</v>
       </c>
-      <c r="L27" s="2" t="n">
+      <c r="L27" s="3" t="n">
         <v>36.22</v>
       </c>
-      <c r="M27" s="2" t="n">
+      <c r="M27" s="3" t="n">
         <v>2.59</v>
       </c>
-      <c r="O27" s="2" t="n">
+      <c r="O27" s="3" t="n">
         <v>8.329984877</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q27" s="2" t="n">
+      <c r="P27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q27" s="3" t="n">
         <v>32.03</v>
       </c>
-      <c r="R27" s="2" t="n">
+      <c r="R27" s="3" t="n">
         <v>6.406</v>
       </c>
-      <c r="S27" s="2" t="n">
+      <c r="S27" s="3" t="n">
         <v>4.037182352</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D28" s="1" t="n">
+      <c r="C28" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D28" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="E28" s="3" t="n">
+      <c r="E28" s="4" t="n">
         <v>70</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="3" t="n">
         <v>-24.96</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="3" t="n">
         <v>164.51</v>
       </c>
-      <c r="H28" s="2" t="n">
+      <c r="H28" s="3" t="n">
         <v>0.16</v>
       </c>
-      <c r="I28" s="2" t="n">
+      <c r="I28" s="3" t="n">
         <v>13.7</v>
       </c>
-      <c r="K28" s="2" t="n">
+      <c r="K28" s="3" t="n">
         <v>8.37</v>
       </c>
-      <c r="L28" s="2" t="n">
+      <c r="L28" s="3" t="n">
         <v>23.6</v>
       </c>
-      <c r="M28" s="2" t="n">
+      <c r="M28" s="3" t="n">
         <v>1.68</v>
       </c>
-      <c r="O28" s="2" t="n">
+      <c r="O28" s="3" t="n">
         <v>8.130971112</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="2" t="n">
+      <c r="P28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="3" t="n">
         <v>31.74</v>
       </c>
-      <c r="R28" s="2" t="n">
+      <c r="R28" s="3" t="n">
         <v>6.348</v>
       </c>
-      <c r="S28" s="2" t="n">
+      <c r="S28" s="3" t="n">
         <v>2.59152113</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D29" s="1" t="n">
+      <c r="C29" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D29" s="2" t="n">
         <v>710</v>
       </c>
-      <c r="E29" s="3" t="n">
+      <c r="E29" s="4" t="n">
         <v>710</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="3" t="n">
         <v>-22.88</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="3" t="n">
         <v>134.61</v>
       </c>
-      <c r="H29" s="2" t="n">
+      <c r="H29" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I29" s="2" t="n">
+      <c r="I29" s="3" t="n">
         <v>11.21</v>
       </c>
-      <c r="K29" s="2" t="n">
+      <c r="K29" s="3" t="n">
         <v>11.08</v>
       </c>
-      <c r="L29" s="2" t="n">
+      <c r="L29" s="3" t="n">
         <v>19.18</v>
       </c>
-      <c r="M29" s="2" t="n">
+      <c r="M29" s="3" t="n">
         <v>1.37</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="N29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O29" s="2" t="n">
+      <c r="O29" s="3" t="n">
         <v>8.186815523</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="2" t="n">
+      <c r="P29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="3" t="n">
         <v>33.28</v>
       </c>
-      <c r="R29" s="2" t="n">
+      <c r="R29" s="3" t="n">
         <v>6.656</v>
       </c>
-      <c r="S29" s="2" t="n">
+      <c r="S29" s="3" t="n">
         <v>2.022361923</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D30" s="1" t="n">
+      <c r="C30" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D30" s="2" t="n">
         <v>350</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="4" t="n">
         <v>350</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="3" t="n">
         <v>-24.15</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="3" t="n">
         <v>154.73</v>
       </c>
-      <c r="H30" s="2" t="n">
+      <c r="H30" s="3" t="n">
         <v>0.15</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="I30" s="3" t="n">
         <v>12.88</v>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="K30" s="3" t="n">
         <v>9.41</v>
       </c>
-      <c r="L30" s="2" t="n">
+      <c r="L30" s="3" t="n">
         <v>21.62</v>
       </c>
-      <c r="M30" s="2" t="n">
+      <c r="M30" s="3" t="n">
         <v>1.54</v>
       </c>
-      <c r="O30" s="2" t="n">
+      <c r="O30" s="3" t="n">
         <v>8.349918235</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q30" s="2" t="n">
+      <c r="P30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="3" t="n">
         <v>32.5</v>
       </c>
-      <c r="R30" s="2" t="n">
+      <c r="R30" s="3" t="n">
         <v>6.5</v>
       </c>
-      <c r="S30" s="2" t="n">
+      <c r="S30" s="3" t="n">
         <v>2.380499619</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D31" s="1" t="n">
+      <c r="C31" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D31" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="F31" s="2" t="n">
+      <c r="F31" s="3" t="n">
         <v>-25.03</v>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G31" s="3" t="n">
         <v>361.75</v>
       </c>
-      <c r="H31" s="2" t="n">
+      <c r="H31" s="3" t="n">
         <v>0.36</v>
       </c>
-      <c r="I31" s="2" t="n">
+      <c r="I31" s="3" t="n">
         <v>30.12</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="K31" s="3" t="n">
         <v>9.6</v>
       </c>
-      <c r="L31" s="2" t="n">
+      <c r="L31" s="3" t="n">
         <v>52.31</v>
       </c>
-      <c r="M31" s="2" t="n">
+      <c r="M31" s="3" t="n">
         <v>3.73</v>
       </c>
-      <c r="O31" s="2" t="n">
+      <c r="O31" s="3" t="n">
         <v>8.067341675</v>
       </c>
-      <c r="P31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q31" s="2" t="n">
+      <c r="P31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q31" s="3" t="n">
         <v>39.23</v>
       </c>
-      <c r="R31" s="2" t="n">
+      <c r="R31" s="3" t="n">
         <v>7.846</v>
       </c>
-      <c r="S31" s="2" t="n">
+      <c r="S31" s="3" t="n">
         <v>4.61068689</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D32" s="1" t="n">
+      <c r="C32" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D32" s="2" t="n">
         <v>250</v>
       </c>
-      <c r="E32" s="3" t="n">
+      <c r="E32" s="4" t="n">
         <v>250</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F32" s="3" t="n">
         <v>-23.59</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G32" s="3" t="n">
         <v>268.01</v>
       </c>
-      <c r="H32" s="2" t="n">
+      <c r="H32" s="3" t="n">
         <v>0.27</v>
       </c>
-      <c r="I32" s="2" t="n">
+      <c r="I32" s="3" t="n">
         <v>22.32</v>
       </c>
-      <c r="K32" s="2" t="n">
+      <c r="K32" s="3" t="n">
         <v>9.46</v>
       </c>
-      <c r="L32" s="2" t="n">
+      <c r="L32" s="3" t="n">
         <v>51.68</v>
       </c>
-      <c r="M32" s="2" t="n">
+      <c r="M32" s="3" t="n">
         <v>3.69</v>
       </c>
-      <c r="O32" s="2" t="n">
+      <c r="O32" s="3" t="n">
         <v>6.049367233</v>
       </c>
-      <c r="P32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q32" s="2" t="n">
+      <c r="P32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q32" s="3" t="n">
         <v>41.79</v>
       </c>
-      <c r="R32" s="2" t="n">
+      <c r="R32" s="3" t="n">
         <v>8.358</v>
       </c>
-      <c r="S32" s="2" t="n">
+      <c r="S32" s="3" t="n">
         <v>3.206575198</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D33" s="1" t="n">
+      <c r="C33" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D33" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="E33" s="3" t="n">
+      <c r="E33" s="4" t="n">
         <v>110</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F33" s="3" t="n">
         <v>-24.54</v>
       </c>
-      <c r="G33" s="2" t="n">
+      <c r="G33" s="3" t="n">
         <v>343.02</v>
       </c>
-      <c r="H33" s="2" t="n">
+      <c r="H33" s="3" t="n">
         <v>0.34</v>
       </c>
-      <c r="I33" s="2" t="n">
+      <c r="I33" s="3" t="n">
         <v>28.56</v>
       </c>
-      <c r="K33" s="2" t="n">
+      <c r="K33" s="3" t="n">
         <v>9.53</v>
       </c>
-      <c r="L33" s="2" t="n">
+      <c r="L33" s="3" t="n">
         <v>47.55</v>
       </c>
-      <c r="M33" s="2" t="n">
+      <c r="M33" s="3" t="n">
         <v>3.39</v>
       </c>
-      <c r="O33" s="2" t="n">
+      <c r="O33" s="3" t="n">
         <v>8.415298901</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q33" s="2" t="n">
+      <c r="P33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q33" s="3" t="n">
         <v>38.2</v>
       </c>
-      <c r="R33" s="2" t="n">
+      <c r="R33" s="3" t="n">
         <v>7.64</v>
       </c>
-      <c r="S33" s="2" t="n">
+      <c r="S33" s="3" t="n">
         <v>4.489757161</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D34" s="1" t="n">
+      <c r="C34" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D34" s="2" t="n">
         <v>990</v>
       </c>
-      <c r="E34" s="3" t="n">
+      <c r="E34" s="4" t="n">
         <v>990</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F34" s="3" t="n">
         <v>-22.69</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G34" s="3" t="n">
         <v>92.08</v>
       </c>
-      <c r="H34" s="2" t="n">
+      <c r="H34" s="3" t="n">
         <v>0.09</v>
       </c>
-      <c r="I34" s="2" t="n">
+      <c r="I34" s="3" t="n">
         <v>7.67</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K34" s="2" t="n">
+      <c r="K34" s="3" t="n">
         <v>9.55</v>
       </c>
-      <c r="L34" s="2" t="n">
+      <c r="L34" s="3" t="n">
         <v>13.31</v>
       </c>
-      <c r="M34" s="2" t="n">
+      <c r="M34" s="3" t="n">
         <v>0.95</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="N34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O34" s="2" t="n">
+      <c r="O34" s="3" t="n">
         <v>8.070197101</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q34" s="2" t="n">
+      <c r="P34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="3" t="n">
         <v>36.93</v>
       </c>
-      <c r="R34" s="2" t="n">
+      <c r="R34" s="3" t="n">
         <v>7.386</v>
       </c>
-      <c r="S34" s="2" t="n">
+      <c r="S34" s="3" t="n">
         <v>1.246674811</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D35" s="1" t="n">
+      <c r="C35" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D35" s="2" t="n">
         <v>2500</v>
       </c>
-      <c r="E35" s="3" t="n">
+      <c r="E35" s="4" t="n">
         <v>2500</v>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="F35" s="3" t="n">
         <v>-25.78</v>
       </c>
-      <c r="G35" s="2" t="n">
+      <c r="G35" s="3" t="n">
         <v>17.65</v>
       </c>
-      <c r="H35" s="2" t="n">
+      <c r="H35" s="3" t="n">
         <v>0.02</v>
       </c>
-      <c r="I35" s="2" t="n">
+      <c r="I35" s="3" t="n">
         <v>1.47</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="2" t="n">
+      <c r="K35" s="3" t="n">
         <v>8.58</v>
       </c>
-      <c r="L35" s="2" t="n">
+      <c r="L35" s="3" t="n">
         <v>2.63</v>
       </c>
-      <c r="M35" s="2" t="n">
+      <c r="M35" s="3" t="n">
         <v>0.19</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="N35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O35" s="2" t="n">
+      <c r="O35" s="3" t="n">
         <v>7.830111515</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q35" s="2" t="n">
+      <c r="P35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q35" s="3" t="n">
         <v>35.49</v>
       </c>
-      <c r="R35" s="2" t="n">
+      <c r="R35" s="3" t="n">
         <v>7.098</v>
       </c>
-      <c r="S35" s="2" t="n">
-        <v>0.248672059</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="S35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D36" s="1" t="n">
+      <c r="C36" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D36" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="E36" s="3" t="n">
+      <c r="E36" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="3" t="n">
         <v>-24.97</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="3" t="n">
         <v>335.52</v>
       </c>
-      <c r="H36" s="2" t="n">
+      <c r="H36" s="3" t="n">
         <v>0.34</v>
       </c>
-      <c r="I36" s="2" t="n">
+      <c r="I36" s="3" t="n">
         <v>27.94</v>
       </c>
-      <c r="K36" s="2" t="n">
+      <c r="K36" s="3" t="n">
         <v>9.53</v>
       </c>
-      <c r="L36" s="2" t="n">
+      <c r="L36" s="3" t="n">
         <v>46.29</v>
       </c>
-      <c r="M36" s="2" t="n">
+      <c r="M36" s="3" t="n">
         <v>3.3</v>
       </c>
-      <c r="O36" s="2" t="n">
+      <c r="O36" s="3" t="n">
         <v>8.455085995</v>
       </c>
-      <c r="P36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q36" s="2" t="n">
+      <c r="P36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="3" t="n">
         <v>39.39</v>
       </c>
-      <c r="R36" s="2" t="n">
+      <c r="R36" s="3" t="n">
         <v>7.878</v>
       </c>
-      <c r="S36" s="2" t="n">
+      <c r="S36" s="3" t="n">
         <v>4.258959695</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D37" s="1" t="n">
+      <c r="C37" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D37" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="E37" s="3" t="n">
+      <c r="E37" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="3" t="n">
         <v>-22.94</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G37" s="3" t="n">
         <v>290.52</v>
       </c>
-      <c r="H37" s="2" t="n">
+      <c r="H37" s="3" t="n">
         <v>0.29</v>
       </c>
-      <c r="I37" s="2" t="n">
+      <c r="I37" s="3" t="n">
         <v>24.19</v>
       </c>
-      <c r="K37" s="2" t="n">
+      <c r="K37" s="3" t="n">
         <v>7.94</v>
       </c>
-      <c r="L37" s="2" t="n">
+      <c r="L37" s="3" t="n">
         <v>50.33</v>
       </c>
-      <c r="M37" s="2" t="n">
+      <c r="M37" s="3" t="n">
         <v>3.59</v>
       </c>
-      <c r="O37" s="2" t="n">
+      <c r="O37" s="3" t="n">
         <v>6.733042913</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q37" s="2" t="n">
+      <c r="P37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q37" s="3" t="n">
         <v>36.09</v>
       </c>
-      <c r="R37" s="2" t="n">
+      <c r="R37" s="3" t="n">
         <v>7.218</v>
       </c>
-      <c r="S37" s="2" t="n">
+      <c r="S37" s="3" t="n">
         <v>4.024935237</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D38" s="1" t="n">
+      <c r="C38" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D38" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="E38" s="3" t="n">
+      <c r="E38" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F38" s="3" t="n">
         <v>-25.11</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G38" s="3" t="n">
         <v>358.01</v>
       </c>
-      <c r="H38" s="2" t="n">
+      <c r="H38" s="3" t="n">
         <v>0.36</v>
       </c>
-      <c r="I38" s="2" t="n">
+      <c r="I38" s="3" t="n">
         <v>29.81</v>
       </c>
-      <c r="K38" s="2" t="n">
+      <c r="K38" s="3" t="n">
         <v>8.72</v>
       </c>
-      <c r="L38" s="2" t="n">
+      <c r="L38" s="3" t="n">
         <v>54.55</v>
       </c>
-      <c r="M38" s="2" t="n">
+      <c r="M38" s="3" t="n">
         <v>3.89</v>
       </c>
-      <c r="O38" s="2" t="n">
+      <c r="O38" s="3" t="n">
         <v>7.655364916</v>
       </c>
-      <c r="P38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q38" s="2" t="n">
+      <c r="P38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q38" s="3" t="n">
         <v>34.1</v>
       </c>
-      <c r="R38" s="2" t="n">
+      <c r="R38" s="3" t="n">
         <v>6.82</v>
       </c>
-      <c r="S38" s="2" t="n">
+      <c r="S38" s="3" t="n">
         <v>5.249378208</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D39" s="1" t="n">
+      <c r="C39" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D39" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="E39" s="3" t="n">
+      <c r="E39" s="4" t="n">
         <v>90</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F39" s="3" t="n">
         <v>-25.85</v>
       </c>
-      <c r="G39" s="2" t="n">
+      <c r="G39" s="3" t="n">
         <v>247.36</v>
       </c>
-      <c r="H39" s="2" t="n">
+      <c r="H39" s="3" t="n">
         <v>0.25</v>
       </c>
-      <c r="I39" s="2" t="n">
+      <c r="I39" s="3" t="n">
         <v>20.6</v>
       </c>
-      <c r="K39" s="2" t="n">
+      <c r="K39" s="3" t="n">
         <v>9.78</v>
       </c>
-      <c r="L39" s="2" t="n">
+      <c r="L39" s="3" t="n">
         <v>35.32</v>
       </c>
-      <c r="M39" s="2" t="n">
+      <c r="M39" s="3" t="n">
         <v>2.52</v>
       </c>
-      <c r="O39" s="2" t="n">
+      <c r="O39" s="3" t="n">
         <v>8.170318199</v>
       </c>
-      <c r="P39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q39" s="2" t="n">
+      <c r="P39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="R39" s="2" t="n">
+      <c r="R39" s="3" t="n">
         <v>6.2</v>
       </c>
-      <c r="S39" s="2" t="n">
+      <c r="S39" s="3" t="n">
         <v>3.989667983</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D40" s="1" t="n">
+      <c r="C40" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D40" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="E40" s="3" t="n">
+      <c r="E40" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F40" s="3" t="n">
         <v>-25.35</v>
       </c>
-      <c r="G40" s="2" t="n">
+      <c r="G40" s="3" t="n">
         <v>133.29</v>
       </c>
-      <c r="H40" s="2" t="n">
+      <c r="H40" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I40" s="2" t="n">
+      <c r="I40" s="3" t="n">
         <v>11.1</v>
       </c>
-      <c r="K40" s="2" t="n">
+      <c r="K40" s="3" t="n">
         <v>9.76</v>
       </c>
-      <c r="L40" s="2" t="n">
+      <c r="L40" s="3" t="n">
         <v>18.46</v>
       </c>
-      <c r="M40" s="2" t="n">
+      <c r="M40" s="3" t="n">
         <v>1.32</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O40" s="2" t="n">
+      <c r="O40" s="3" t="n">
         <v>8.423917643</v>
       </c>
-      <c r="P40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q40" s="2" t="n">
+      <c r="P40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q40" s="3" t="n">
         <v>32.1</v>
       </c>
-      <c r="R40" s="2" t="n">
+      <c r="R40" s="3" t="n">
         <v>6.42</v>
       </c>
-      <c r="S40" s="2" t="n">
+      <c r="S40" s="3" t="n">
         <v>2.076193579</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D41" s="1" t="n">
+      <c r="C41" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D41" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="F41" s="3" t="n">
         <v>-25.01</v>
       </c>
-      <c r="G41" s="2" t="n">
+      <c r="G41" s="3" t="n">
         <v>258.62</v>
       </c>
-      <c r="H41" s="2" t="n">
+      <c r="H41" s="3" t="n">
         <v>0.26</v>
       </c>
-      <c r="I41" s="2" t="n">
+      <c r="I41" s="3" t="n">
         <v>21.53</v>
       </c>
-      <c r="K41" s="2" t="n">
+      <c r="K41" s="3" t="n">
         <v>10.98</v>
       </c>
-      <c r="L41" s="2" t="n">
+      <c r="L41" s="3" t="n">
         <v>34.15</v>
       </c>
-      <c r="M41" s="2" t="n">
+      <c r="M41" s="3" t="n">
         <v>2.44</v>
       </c>
-      <c r="O41" s="2" t="n">
+      <c r="O41" s="3" t="n">
         <v>8.835144659</v>
       </c>
-      <c r="P41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q41" s="2" t="n">
+      <c r="P41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q41" s="3" t="n">
         <v>32.2</v>
       </c>
-      <c r="R41" s="2" t="n">
+      <c r="R41" s="3" t="n">
         <v>6.44</v>
       </c>
-      <c r="S41" s="2" t="n">
+      <c r="S41" s="3" t="n">
         <v>4.015868036</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D42" s="1" t="n">
+      <c r="C42" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D42" s="2" t="n">
         <v>2000</v>
       </c>
-      <c r="E42" s="3" t="n">
+      <c r="E42" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F42" s="3" t="n">
         <v>-23.07</v>
       </c>
-      <c r="G42" s="2" t="n">
+      <c r="G42" s="3" t="n">
         <v>128.21</v>
       </c>
-      <c r="H42" s="2" t="n">
+      <c r="H42" s="3" t="n">
         <v>0.13</v>
       </c>
-      <c r="I42" s="2" t="n">
+      <c r="I42" s="3" t="n">
         <v>10.68</v>
       </c>
-      <c r="K42" s="2" t="n">
+      <c r="K42" s="3" t="n">
         <v>9.95</v>
       </c>
-      <c r="L42" s="2" t="n">
+      <c r="L42" s="3" t="n">
         <v>16.47</v>
       </c>
-      <c r="M42" s="2" t="n">
+      <c r="M42" s="3" t="n">
         <v>1.18</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="N42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O42" s="2" t="n">
+      <c r="O42" s="3" t="n">
         <v>9.080128433</v>
       </c>
-      <c r="P42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q42" s="2" t="n">
+      <c r="P42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q42" s="3" t="n">
         <v>32.5</v>
       </c>
-      <c r="R42" s="2" t="n">
+      <c r="R42" s="3" t="n">
         <v>6.5</v>
       </c>
-      <c r="S42" s="2" t="n">
+      <c r="S42" s="3" t="n">
         <v>1.972497226</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D43" s="1" t="n">
+      <c r="C43" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D43" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="E43" s="3" t="n">
+      <c r="E43" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="F43" s="2" t="n">
+      <c r="F43" s="3" t="n">
         <v>-26.82</v>
       </c>
-      <c r="G43" s="2" t="n">
+      <c r="G43" s="3" t="n">
         <v>198.53</v>
       </c>
-      <c r="H43" s="2" t="n">
+      <c r="H43" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="I43" s="2" t="n">
+      <c r="I43" s="3" t="n">
         <v>16.53</v>
       </c>
-      <c r="K43" s="2" t="n">
+      <c r="K43" s="3" t="n">
         <v>17.54</v>
       </c>
-      <c r="L43" s="2" t="n">
+      <c r="L43" s="3" t="n">
         <v>20.26</v>
       </c>
-      <c r="M43" s="2" t="n">
+      <c r="M43" s="3" t="n">
         <v>1.45</v>
       </c>
-      <c r="O43" s="2" t="n">
+      <c r="O43" s="3" t="n">
         <v>11.42900726</v>
       </c>
-      <c r="P43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q43" s="2" t="n">
+      <c r="P43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q43" s="3" t="n">
         <v>31.2</v>
       </c>
-      <c r="R43" s="2" t="n">
+      <c r="R43" s="3" t="n">
         <v>6.24</v>
       </c>
-      <c r="S43" s="2" t="n">
+      <c r="S43" s="3" t="n">
         <v>3.181551353</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D44" s="1" t="n">
+      <c r="C44" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D44" s="2" t="n">
         <v>1600</v>
       </c>
-      <c r="E44" s="3" t="n">
+      <c r="E44" s="4" t="n">
         <v>1600</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="3" t="n">
         <v>-24.1</v>
       </c>
-      <c r="G44" s="2" t="n">
+      <c r="G44" s="3" t="n">
         <v>71.18</v>
       </c>
-      <c r="H44" s="2" t="n">
+      <c r="H44" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="I44" s="2" t="n">
+      <c r="I44" s="3" t="n">
         <v>5.93</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="J44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="2" t="n">
+      <c r="K44" s="3" t="n">
         <v>9.2</v>
       </c>
-      <c r="L44" s="2" t="n">
+      <c r="L44" s="3" t="n">
         <v>9.15</v>
       </c>
-      <c r="M44" s="2" t="n">
+      <c r="M44" s="3" t="n">
         <v>0.65</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N44" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O44" s="2" t="n">
+      <c r="O44" s="3" t="n">
         <v>9.072530509</v>
       </c>
-      <c r="P44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q44" s="2" t="n">
+      <c r="P44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q44" s="3" t="n">
         <v>33.6</v>
       </c>
-      <c r="R44" s="2" t="n">
+      <c r="R44" s="3" t="n">
         <v>6.72</v>
       </c>
-      <c r="S44" s="2" t="n">
+      <c r="S44" s="3" t="n">
         <v>1.059216444</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="1" t="n">
-        <v>2012</v>
-      </c>
-      <c r="D45" s="1" t="n">
+      <c r="C45" s="2" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D45" s="2" t="n">
         <v>1300</v>
       </c>
-      <c r="E45" s="3" t="n">
+      <c r="E45" s="4" t="n">
         <v>1300</v>
       </c>
-      <c r="F45" s="2" t="n">
+      <c r="F45" s="3" t="n">
         <v>-23.61</v>
       </c>
-      <c r="G45" s="2" t="n">
+      <c r="G45" s="3" t="n">
         <v>144.77</v>
       </c>
-      <c r="H45" s="2" t="n">
+      <c r="H45" s="3" t="n">
         <v>0.14</v>
       </c>
-      <c r="I45" s="2" t="n">
+      <c r="I45" s="3" t="n">
         <v>12.05</v>
       </c>
-      <c r="K45" s="2" t="n">
+      <c r="K45" s="3" t="n">
         <v>12.08</v>
       </c>
-      <c r="L45" s="2" t="n">
+      <c r="L45" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="M45" s="2" t="n">
+      <c r="M45" s="3" t="n">
         <v>1.36</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="N45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O45" s="2" t="n">
+      <c r="O45" s="3" t="n">
         <v>8.888222033</v>
       </c>
-      <c r="P45" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q45" s="2" t="n">
+      <c r="P45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="R45" s="2" t="n">
+      <c r="R45" s="3" t="n">
         <v>7.2</v>
       </c>
-      <c r="S45" s="2" t="n">
+      <c r="S45" s="3" t="n">
         <v>2.010630441</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plotted 2019 stable isos in with the suspended
</commit_message>
<xml_diff>
--- a/data/flux/2012-pumps.xlsx
+++ b/data/flux/2012-pumps.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">d15N Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">C:N </t>
+    <t xml:space="preserve">C:N</t>
   </si>
   <si>
     <t xml:space="preserve">Tray Name</t>
@@ -370,13 +370,13 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
old calc of sus conc c 2017
</commit_message>
<xml_diff>
--- a/data/flux/2012-pumps.xlsx
+++ b/data/flux/2012-pumps.xlsx
@@ -369,11 +369,11 @@
   </sheetPr>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="14.43"/>
@@ -2819,7 +2819,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>